<commit_message>
Modify cost reports to match reports API
</commit_message>
<xml_diff>
--- a/storage/templates/cost-summary.xlsx
+++ b/storage/templates/cost-summary.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hazem/apps/cost-control/storage/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\code\cost-control\storage\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Summary" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,11 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -101,16 +101,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(#,##0.00_);_(\(#,##0.00\);_(&quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(#,##0.00_);_(\(#,##0.00\);_(&quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -118,21 +118,21 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -140,7 +140,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -148,7 +148,7 @@
       <b/>
       <sz val="14"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -330,36 +330,36 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="5" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -368,16 +368,16 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -678,29 +678,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="19.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.25" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
@@ -715,7 +715,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
@@ -730,7 +730,7 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
@@ -745,7 +745,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>20</v>
       </c>
@@ -760,7 +760,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
@@ -775,7 +775,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -816,7 +816,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>0</v>
       </c>
@@ -842,7 +842,7 @@
       <c r="K9" s="20"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="8" t="s">
         <v>2</v>
@@ -875,7 +875,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -888,7 +888,7 @@
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -901,7 +901,7 @@
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -914,7 +914,7 @@
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -927,7 +927,7 @@
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -940,7 +940,7 @@
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -953,7 +953,7 @@
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -966,7 +966,7 @@
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>

</xml_diff>

<commit_message>
Re-adjust cost summary report
</commit_message>
<xml_diff>
--- a/storage/templates/cost-summary.xlsx
+++ b/storage/templates/cost-summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10513"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hazem/code/cost-control/storage/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23296A5E-DCEE-BD44-B3F8-27349BEE72F3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EF74F3-98F2-944E-BD83-315F60D5920D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Resource Type</t>
   </si>
@@ -46,12 +46,6 @@
   </si>
   <si>
     <t>Previous Cost</t>
-  </si>
-  <si>
-    <t>Previous (EV) Allowable</t>
-  </si>
-  <si>
-    <t>Previous Variance</t>
   </si>
   <si>
     <t>Todate Cost</t>
@@ -177,7 +171,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -287,17 +281,6 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="medium">
-        <color theme="0"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -334,14 +317,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="1" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="1" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -357,29 +340,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="5" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="5" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="2" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -679,7 +659,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
@@ -687,22 +667,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="27.1640625" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.83203125" customWidth="1"/>
-    <col min="10" max="10" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.5" customWidth="1"/>
+    <col min="2" max="9" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -712,12 +683,10 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -727,12 +696,10 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -742,12 +709,10 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -757,12 +722,10 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -772,25 +735,21 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" ht="19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:10" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
+      <c r="D6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -800,10 +759,8 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -813,204 +770,170 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+    </row>
+    <row r="9" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="15" t="s">
+      <c r="D9" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="18"/>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
       <c r="B10" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="7" t="s">
+      <c r="G10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="D6:H6"/>
+  <mergeCells count="4">
+    <mergeCell ref="D6:F6"/>
     <mergeCell ref="A9:A10"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="H9:I9"/>
   </mergeCells>
-  <conditionalFormatting sqref="E11:E18">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H11:H18">
+  <conditionalFormatting sqref="F11:F18">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K11:K18">
+  <conditionalFormatting sqref="I11:I18">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>